<commit_message>
* Updated News Filter
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -675,7 +675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1670,11 +1672,15 @@
       <c r="W12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="X12" s="7"/>
+      <c r="X12" s="7">
+        <v>10</v>
+      </c>
       <c r="Y12" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="Z12" s="7"/>
+      <c r="Z12" s="7">
+        <v>12</v>
+      </c>
       <c r="AA12" s="4" t="s">
         <v>83</v>
       </c>
@@ -1752,11 +1758,15 @@
       <c r="W13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="X13" s="4"/>
+      <c r="X13" s="4">
+        <v>10</v>
+      </c>
       <c r="Y13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="Z13" s="4"/>
+      <c r="Z13" s="4">
+        <v>11</v>
+      </c>
       <c r="AA13" s="4" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
* Fixed a bug with obligatory news not being properly added to lists + Added ending of Caranchotty timeline
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="92">
   <si>
     <t>"Paro de gallos madrugadores"</t>
   </si>
@@ -268,6 +268,30 @@
   </si>
   <si>
     <t>}</t>
+  </si>
+  <si>
+    <t>"Corre riesgo la libertad de prensa"</t>
+  </si>
+  <si>
+    <t>"Fuentes cercanas al gobierno revelaron el plan de expropiación de los medios opositores. Alerta en organismos de libertad de prensa."</t>
+  </si>
+  <si>
+    <t>"Caranchotti vuelve a las andadas"</t>
+  </si>
+  <si>
+    <t>"Se esparce foto de Caranchotti desplumado en lujoso hotel."</t>
+  </si>
+  <si>
+    <t>"El último vuelo"</t>
+  </si>
+  <si>
+    <t>"Caranchotti in fraganti recostado sobre maple de huevos. Impunidad total en altos funcionarios del gobierno"</t>
+  </si>
+  <si>
+    <t>"Caranchotti renuncia tras reiterados escándalos. Me hicieron un nido, graznó fuertemente. Alivio en el gobierno."</t>
+  </si>
+  <si>
+    <t>"Escándalo por docena"</t>
   </si>
 </sst>
 </file>
@@ -359,7 +383,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -368,6 +392,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -673,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1796,7 +1822,7 @@
       <c r="G14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="5" t="s">
@@ -1960,7 +1986,7 @@
       <c r="G16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I16" s="5" t="s">
@@ -2042,7 +2068,7 @@
       <c r="G17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I17" s="5" t="s">
@@ -2288,7 +2314,7 @@
       <c r="G20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I20" s="5" t="s">
@@ -2452,7 +2478,7 @@
       <c r="G22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I22" s="5" t="s">
@@ -2534,7 +2560,7 @@
       <c r="G23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I23" s="5" t="s">
@@ -2616,7 +2642,7 @@
       <c r="G24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I24" s="5" t="s">
@@ -3026,7 +3052,7 @@
       <c r="G29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I29" s="5" t="s">
@@ -3247,6 +3273,344 @@
         <v>83</v>
       </c>
       <c r="AB31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J32" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32" s="6">
+        <v>-0.01</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P32" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R32" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T32" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V32" s="6">
+        <v>10</v>
+      </c>
+      <c r="W32" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="X32" s="6"/>
+      <c r="Y32" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z32" s="6"/>
+      <c r="AA32" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J33" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L33" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N33" s="6">
+        <v>-0.01</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P33" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R33" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T33" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V33" s="6">
+        <v>0</v>
+      </c>
+      <c r="W33" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="X33" s="6">
+        <v>12</v>
+      </c>
+      <c r="Y33" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z33" s="6"/>
+      <c r="AA33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J34" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L34" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P34" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R34" s="7">
+        <v>-0.05</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="T34" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="V34" s="7">
+        <v>0</v>
+      </c>
+      <c r="W34" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="X34" s="7">
+        <v>32</v>
+      </c>
+      <c r="Y34" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z34" s="7">
+        <v>34</v>
+      </c>
+      <c r="AA34" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J35" s="4">
+        <v>-0.04</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L35" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N35" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P35" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R35" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T35" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V35" s="4">
+        <v>0</v>
+      </c>
+      <c r="W35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="X35" s="4">
+        <v>32</v>
+      </c>
+      <c r="Y35" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z35" s="4">
+        <v>33</v>
+      </c>
+      <c r="AA35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB35" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Fixed event order * Fixed formulas
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -912,7 +912,7 @@
       <c r="G3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -994,7 +994,7 @@
       <c r="G4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -1076,7 +1076,7 @@
       <c r="G5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -1158,7 +1158,7 @@
       <c r="G6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -1240,7 +1240,7 @@
       <c r="G7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I7" s="6" t="s">
@@ -1322,7 +1322,7 @@
       <c r="G8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -1404,7 +1404,7 @@
       <c r="G9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -1486,7 +1486,7 @@
       <c r="G10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1568,7 +1568,7 @@
       <c r="G11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -1650,7 +1650,7 @@
       <c r="G12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="9" t="s">
         <v>70</v>
       </c>
       <c r="I12" s="7" t="s">
@@ -1904,7 +1904,7 @@
       <c r="G15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="9" t="s">
         <v>70</v>
       </c>
       <c r="I15" s="7" t="s">
@@ -2150,7 +2150,7 @@
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="9" t="s">
         <v>70</v>
       </c>
       <c r="I18" s="7" t="s">
@@ -2232,7 +2232,7 @@
       <c r="G19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="9" t="s">
         <v>70</v>
       </c>
       <c r="I19" s="7" t="s">
@@ -2396,7 +2396,7 @@
       <c r="G21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I21" s="6" t="s">
@@ -2724,7 +2724,7 @@
       <c r="G25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I25" s="6" t="s">
@@ -2806,7 +2806,7 @@
       <c r="G26" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -2888,7 +2888,7 @@
       <c r="G27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I27" s="6" t="s">
@@ -3625,7 +3625,7 @@
   <dimension ref="B6:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3666,8 +3666,8 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>-1/3+4/3*B10</f>
-        <v>-0.33333333333333331</v>
+        <f>-1/2+3/2*B10</f>
+        <v>-0.5</v>
       </c>
       <c r="D10" s="2">
         <f>B10</f>
@@ -3679,8 +3679,8 @@
         <v>0.1</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C20" si="0">-1/3+4/3*B11</f>
-        <v>-0.19999999999999998</v>
+        <f t="shared" ref="C11:C20" si="0">-1/2+3/2*B11</f>
+        <v>-0.35</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ref="D11:D20" si="1">B11</f>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>-6.6666666666666652E-2</v>
+        <v>-0.19999999999999996</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
@@ -3706,7 +3706,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>6.6666666666666652E-2</v>
+        <v>-5.0000000000000044E-2</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
@@ -3732,7 +3732,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.46666666666666662</v>
+        <v>0.39999999999999991</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
@@ -3758,7 +3758,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.59999999999999987</v>
+        <v>0.54999999999999982</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.73333333333333339</v>
+        <v>0.70000000000000018</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.8666666666666667</v>
+        <v>0.85000000000000009</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
* Some government-positive news
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="138">
   <si>
     <t>"Paro de gallos madrugadores"</t>
   </si>
@@ -180,9 +180,6 @@
     <t>"Ansiedad"</t>
   </si>
   <si>
-    <t>"Faltan 254 días para la época migratoria estival."</t>
-  </si>
-  <si>
     <t>"Ganan los Carroñeros"</t>
   </si>
   <si>
@@ -292,6 +289,147 @@
   </si>
   <si>
     <t>"Escándalo por docena"</t>
+  </si>
+  <si>
+    <t>"Halcones Campeones"</t>
+  </si>
+  <si>
+    <t>"Halcones bajados de un gomerazo"</t>
+  </si>
+  <si>
+    <t>"El equipo de los halcones pierde la final del mundial de garraball, nunca vi tantos pechofrios juntos, refunfuño un fan"</t>
+  </si>
+  <si>
+    <t>"Los Halcones son los campeones indiscutidos del mundial de garraball, algarabío infinito"</t>
+  </si>
+  <si>
+    <t>"Ansiedad Invernal"</t>
+  </si>
+  <si>
+    <t>"Faltan 364 días para la época migratoria estival."</t>
+  </si>
+  <si>
+    <t>"Ansiedad Otoñal"</t>
+  </si>
+  <si>
+    <t>"Ansiedad Primaveral"</t>
+  </si>
+  <si>
+    <t>"Faltan 183 días para el frío."</t>
+  </si>
+  <si>
+    <t>"Faltan 123 días para la caída de hojas."</t>
+  </si>
+  <si>
+    <t>"Faltan 274 días para las flores."</t>
+  </si>
+  <si>
+    <t>"Ganan los Palomos"</t>
+  </si>
+  <si>
+    <t>"El Cardenal"</t>
+  </si>
+  <si>
+    <t>"La película mas taquillera de Gilgero Manso."</t>
+  </si>
+  <si>
+    <t>"El ultimo Faisán"</t>
+  </si>
+  <si>
+    <t>"La galardonada serie ahora en la pantalla grande."</t>
+  </si>
+  <si>
+    <t>"Pulp Pingüin"</t>
+  </si>
+  <si>
+    <t>"1:30 hs de pura adrenalina."</t>
+  </si>
+  <si>
+    <t>"Los aleteos del Colibrí"</t>
+  </si>
+  <si>
+    <t>"Un frenético drama de un amor prohibido."</t>
+  </si>
+  <si>
+    <t>"Tras un intenso enfrentamiento, los Palomos Mensajeros vencen a los Carroñeros por 8 a 5."</t>
+  </si>
+  <si>
+    <t>"Siempre nos respetamos"</t>
+  </si>
+  <si>
+    <t>"La Garza Giménes declaro que aunque haya diferencias siempre se respetaron con la Urraca. Se calman las aguas de los radiopasillos."</t>
+  </si>
+  <si>
+    <t>"Se cuelga de mis alas"</t>
+  </si>
+  <si>
+    <t>"Urraca Casandra desmiente la falsa calma que aparenta la Garza y sostiene, es mas berreta que alpiste de gallinero."</t>
+  </si>
+  <si>
+    <t>"Giménes se defiende"</t>
+  </si>
+  <si>
+    <t>"Hace rato que nadie le arrastra el ala a la Urraca, sostiene desde el estudio."</t>
+  </si>
+  <si>
+    <t>"Divas y algo más"</t>
+  </si>
+  <si>
+    <t>"Avistaron a La Garza Giménes y a la Urraca Casandra a los besos en la playa del Pato Lucas,  estaban mas calientes que la arena dijo una Paloma que pasaba."</t>
+  </si>
+  <si>
+    <t>"Justicia por Roberto"</t>
+  </si>
+  <si>
+    <t>"Marchan las palomas por el asesinato de Roberto Picchotti, el hornero constructor."</t>
+  </si>
+  <si>
+    <t>"Los Picchotti piden a gritos"</t>
+  </si>
+  <si>
+    <t>"La familia de Roberto Picchotti reclaman justicia al gobierno y que se hagan cargo de lo que hicieron."</t>
+  </si>
+  <si>
+    <t>"Reunión de manifestantes"</t>
+  </si>
+  <si>
+    <t>"Se reunen pajaros de todo tipo por el encubrimiento del asesinato de Roberto por parte del gobierno."</t>
+  </si>
+  <si>
+    <t>26,49,50</t>
+  </si>
+  <si>
+    <t>26,49</t>
+  </si>
+  <si>
+    <t>"Se clausuran las sesiones del congreso a la fuerza, Pajaronia acongojada."</t>
+  </si>
+  <si>
+    <t>"Dictador clausura el congreso"</t>
+  </si>
+  <si>
+    <t>"Congreso traidor obtiene su merecido"</t>
+  </si>
+  <si>
+    <t>"El Presidente General Albatros clausura las sesiones del traidor Congreso. Pueblo festeja. Diputados enviados a sus casa."</t>
+  </si>
+  <si>
+    <t>"Presidente Albatros nacionaliza YLF"</t>
+  </si>
+  <si>
+    <t>"Yacimientos Lombricisticos Fiscales vuelve a ser del pueblo, tras 50 años de estas en manos extranjeras."</t>
+  </si>
+  <si>
+    <t>"Fondos Buitres amenazan a Pajaronia"</t>
+  </si>
+  <si>
+    <t>"Fondos Buitres amenazan a Pajaronia, pero el presidente Albatros contesta que jamás pagaremos a los buitres."</t>
+  </si>
+  <si>
+    <t>"Presidente propone nueva bandera"</t>
+  </si>
+  <si>
+    <t>"El presidente Albatros propone una nueva bandera para Pajaronia. Es un hermoso diseño."</t>
   </si>
 </sst>
 </file>
@@ -699,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB35"/>
+  <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -733,7 +871,7 @@
         <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
@@ -751,7 +889,7 @@
         <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
         <v>35</v>
@@ -793,19 +931,19 @@
         <v>35</v>
       </c>
       <c r="V1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W1" t="s">
         <v>35</v>
       </c>
       <c r="X1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" t="s">
         <v>79</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
@@ -831,7 +969,7 @@
         <v>35</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>35</v>
@@ -876,15 +1014,15 @@
         <v>1</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X2" s="4"/>
       <c r="Y2" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB2" t="s">
         <v>38</v>
@@ -913,7 +1051,7 @@
         <v>35</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>35</v>
@@ -958,15 +1096,15 @@
         <v>1</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X3" s="6"/>
       <c r="Y3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z3" s="6"/>
       <c r="AA3" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB3" t="s">
         <v>38</v>
@@ -989,13 +1127,13 @@
         <v>35</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>35</v>
@@ -1040,15 +1178,15 @@
         <v>1</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X4" s="5"/>
       <c r="Y4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z4" s="5"/>
       <c r="AA4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB4" t="s">
         <v>38</v>
@@ -1077,7 +1215,7 @@
         <v>35</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>35</v>
@@ -1122,15 +1260,15 @@
         <v>0</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X5" s="6"/>
       <c r="Y5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z5" s="6"/>
       <c r="AA5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB5" t="s">
         <v>38</v>
@@ -1159,7 +1297,7 @@
         <v>35</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>35</v>
@@ -1204,15 +1342,15 @@
         <v>0</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X6" s="6"/>
       <c r="Y6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z6" s="6"/>
       <c r="AA6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB6" t="s">
         <v>38</v>
@@ -1241,7 +1379,7 @@
         <v>35</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>35</v>
@@ -1286,15 +1424,15 @@
         <v>0</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X7" s="6"/>
       <c r="Y7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z7" s="6"/>
       <c r="AA7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB7" t="s">
         <v>38</v>
@@ -1317,13 +1455,13 @@
         <v>35</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>35</v>
@@ -1368,15 +1506,15 @@
         <v>0</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X8" s="5"/>
       <c r="Y8" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z8" s="5"/>
       <c r="AA8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB8" t="s">
         <v>38</v>
@@ -1405,7 +1543,7 @@
         <v>35</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>35</v>
@@ -1450,15 +1588,15 @@
         <v>0</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X9" s="5"/>
       <c r="Y9" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z9" s="5"/>
       <c r="AA9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB9" t="s">
         <v>38</v>
@@ -1487,7 +1625,7 @@
         <v>35</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>35</v>
@@ -1532,15 +1670,15 @@
         <v>0</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X10" s="5"/>
       <c r="Y10" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z10" s="5"/>
       <c r="AA10" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB10" t="s">
         <v>38</v>
@@ -1569,7 +1707,7 @@
         <v>35</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>35</v>
@@ -1614,15 +1752,15 @@
         <v>0</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X11" s="6"/>
       <c r="Y11" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z11" s="6"/>
       <c r="AA11" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB11" t="s">
         <v>38</v>
@@ -1651,7 +1789,7 @@
         <v>35</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>35</v>
@@ -1696,19 +1834,19 @@
         <v>0</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X12" s="7">
         <v>10</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z12" s="7">
         <v>12</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB12" t="s">
         <v>38</v>
@@ -1737,7 +1875,7 @@
         <v>35</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>35</v>
@@ -1782,19 +1920,19 @@
         <v>0</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X13" s="4">
         <v>10</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z13" s="4">
         <v>11</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB13" t="s">
         <v>38</v>
@@ -1823,7 +1961,7 @@
         <v>35</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>35</v>
@@ -1868,15 +2006,15 @@
         <v>0</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X14" s="5"/>
       <c r="Y14" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z14" s="5"/>
       <c r="AA14" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB14" t="s">
         <v>38</v>
@@ -1905,7 +2043,7 @@
         <v>35</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>35</v>
@@ -1950,15 +2088,15 @@
         <v>0</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X15" s="7"/>
       <c r="Y15" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z15" s="7"/>
       <c r="AA15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB15" t="s">
         <v>38</v>
@@ -1987,7 +2125,7 @@
         <v>35</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>35</v>
@@ -2032,15 +2170,15 @@
         <v>0</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X16" s="5"/>
       <c r="Y16" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z16" s="5"/>
       <c r="AA16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB16" t="s">
         <v>38</v>
@@ -2069,7 +2207,7 @@
         <v>35</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>35</v>
@@ -2114,15 +2252,15 @@
         <v>0</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X17" s="5"/>
       <c r="Y17" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z17" s="5"/>
       <c r="AA17" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB17" t="s">
         <v>38</v>
@@ -2151,7 +2289,7 @@
         <v>35</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>35</v>
@@ -2196,15 +2334,15 @@
         <v>0</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X18" s="7"/>
       <c r="Y18" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z18" s="7"/>
       <c r="AA18" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB18" t="s">
         <v>38</v>
@@ -2233,7 +2371,7 @@
         <v>35</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>35</v>
@@ -2278,15 +2416,15 @@
         <v>0</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X19" s="7"/>
       <c r="Y19" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z19" s="7"/>
       <c r="AA19" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB19" t="s">
         <v>38</v>
@@ -2315,7 +2453,7 @@
         <v>35</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>35</v>
@@ -2360,15 +2498,15 @@
         <v>0</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X20" s="5"/>
       <c r="Y20" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z20" s="5"/>
       <c r="AA20" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB20" t="s">
         <v>38</v>
@@ -2397,7 +2535,7 @@
         <v>35</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>35</v>
@@ -2442,15 +2580,15 @@
         <v>0</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X21" s="6"/>
       <c r="Y21" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z21" s="6"/>
       <c r="AA21" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB21" t="s">
         <v>38</v>
@@ -2473,38 +2611,38 @@
         <v>35</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="J22" s="5">
+        <v>-0.03</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="5">
         <v>-0.02</v>
       </c>
-      <c r="K22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L22" s="5">
-        <v>-0.01</v>
-      </c>
       <c r="M22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N22" s="5">
+        <v>-0.03</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" s="5">
         <v>-0.02</v>
       </c>
-      <c r="O22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P22" s="5">
-        <v>-0.01</v>
-      </c>
       <c r="Q22" s="5" t="s">
         <v>35</v>
       </c>
@@ -2524,15 +2662,15 @@
         <v>0</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X22" s="5"/>
       <c r="Y22" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z22" s="5"/>
       <c r="AA22" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB22" t="s">
         <v>38</v>
@@ -2549,19 +2687,19 @@
         <v>35</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="G23" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>35</v>
@@ -2606,15 +2744,17 @@
         <v>0</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X23" s="5"/>
       <c r="Y23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z23" s="5">
+        <v>40</v>
+      </c>
+      <c r="AA23" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="AB23" t="s">
         <v>38</v>
@@ -2631,19 +2771,19 @@
         <v>35</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>35</v>
@@ -2688,15 +2828,15 @@
         <v>0</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X24" s="5"/>
       <c r="Y24" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z24" s="5"/>
       <c r="AA24" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB24" t="s">
         <v>38</v>
@@ -2713,19 +2853,19 @@
         <v>35</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="G25" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>35</v>
@@ -2770,15 +2910,15 @@
         <v>0</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X25" s="6"/>
       <c r="Y25" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z25" s="6"/>
       <c r="AA25" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB25" t="s">
         <v>38</v>
@@ -2795,19 +2935,19 @@
         <v>35</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="G26" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>35</v>
@@ -2852,15 +2992,15 @@
         <v>0</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X26" s="6"/>
       <c r="Y26" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z26" s="6"/>
       <c r="AA26" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB26" t="s">
         <v>38</v>
@@ -2877,19 +3017,19 @@
         <v>35</v>
       </c>
       <c r="D27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="G27" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>35</v>
@@ -2934,15 +3074,15 @@
         <v>0</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X27" s="6"/>
       <c r="Y27" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z27" s="6"/>
       <c r="AA27" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB27" t="s">
         <v>38</v>
@@ -2959,19 +3099,19 @@
         <v>35</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="G28" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>35</v>
@@ -3016,15 +3156,15 @@
         <v>0</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X28" s="4"/>
       <c r="Y28" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z28" s="4"/>
       <c r="AA28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB28" t="s">
         <v>38</v>
@@ -3041,19 +3181,19 @@
         <v>35</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>35</v>
@@ -3098,15 +3238,15 @@
         <v>0</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X29" s="5"/>
       <c r="Y29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z29" s="5"/>
       <c r="AA29" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB29" t="s">
         <v>38</v>
@@ -3123,19 +3263,19 @@
         <v>35</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="G30" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>35</v>
@@ -3180,15 +3320,15 @@
         <v>0</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X30" s="4"/>
       <c r="Y30" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z30" s="4"/>
       <c r="AA30" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB30" t="s">
         <v>38</v>
@@ -3205,19 +3345,19 @@
         <v>35</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>35</v>
@@ -3262,15 +3402,15 @@
         <v>0</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X31" s="4"/>
       <c r="Y31" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z31" s="4"/>
       <c r="AA31" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB31" t="s">
         <v>38</v>
@@ -3287,19 +3427,19 @@
         <v>35</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="G32" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>35</v>
@@ -3341,18 +3481,20 @@
         <v>35</v>
       </c>
       <c r="V32" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="W32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X32" s="6">
+        <v>52</v>
+      </c>
+      <c r="Y32" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="Z32" s="6"/>
       <c r="AA32" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB32" t="s">
         <v>38</v>
@@ -3369,19 +3511,19 @@
         <v>35</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="G33" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>35</v>
@@ -3426,17 +3568,17 @@
         <v>0</v>
       </c>
       <c r="W33" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X33" s="6">
         <v>12</v>
       </c>
       <c r="Y33" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z33" s="6"/>
       <c r="AA33" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB33" t="s">
         <v>38</v>
@@ -3453,19 +3595,19 @@
         <v>35</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>35</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>35</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>35</v>
@@ -3510,19 +3652,19 @@
         <v>0</v>
       </c>
       <c r="W34" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X34" s="7">
         <v>32</v>
       </c>
       <c r="Y34" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z34" s="7">
         <v>34</v>
       </c>
       <c r="AA34" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB34" t="s">
         <v>38</v>
@@ -3539,19 +3681,19 @@
         <v>35</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>35</v>
@@ -3596,21 +3738,1855 @@
         <v>0</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X35" s="4">
         <v>32</v>
       </c>
       <c r="Y35" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z35" s="4">
         <v>33</v>
       </c>
       <c r="AA35" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J36" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L36" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N36" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P36" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R36" s="5">
+        <v>0</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T36" s="5">
+        <v>0</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V36" s="5">
+        <v>0</v>
+      </c>
+      <c r="W36" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X36" s="5">
+        <v>8</v>
+      </c>
+      <c r="Y36" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z36" s="5">
+        <v>36</v>
+      </c>
+      <c r="AA36" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J37" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L37" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N37" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P37" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="Q37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R37" s="5">
+        <v>0</v>
+      </c>
+      <c r="S37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T37" s="5">
+        <v>0</v>
+      </c>
+      <c r="U37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V37" s="5">
+        <v>0</v>
+      </c>
+      <c r="W37" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X37" s="5">
+        <v>8</v>
+      </c>
+      <c r="Y37" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z37" s="5">
+        <v>35</v>
+      </c>
+      <c r="AA37" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L38" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N38" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P38" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R38" s="5">
+        <v>0</v>
+      </c>
+      <c r="S38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T38" s="5">
+        <v>0</v>
+      </c>
+      <c r="U38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V38" s="5">
+        <v>0</v>
+      </c>
+      <c r="W38" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X38" s="5">
+        <v>39</v>
+      </c>
+      <c r="Y38" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J39" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L39" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N39" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P39" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R39" s="5">
+        <v>0</v>
+      </c>
+      <c r="S39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T39" s="5">
+        <v>0</v>
+      </c>
+      <c r="U39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V39" s="5">
+        <v>0</v>
+      </c>
+      <c r="W39" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X39" s="5">
+        <v>37</v>
+      </c>
+      <c r="Y39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J40" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L40" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N40" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P40" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="Q40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R40" s="5">
+        <v>0</v>
+      </c>
+      <c r="S40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T40" s="5">
+        <v>0</v>
+      </c>
+      <c r="U40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V40" s="5">
+        <v>0</v>
+      </c>
+      <c r="W40" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X40" s="5">
+        <v>21</v>
+      </c>
+      <c r="Y40" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L41" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N41" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P41" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R41" s="5">
+        <v>0</v>
+      </c>
+      <c r="S41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T41" s="5">
+        <v>0</v>
+      </c>
+      <c r="U41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V41" s="5">
+        <v>0</v>
+      </c>
+      <c r="W41" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z41" s="5">
+        <v>22</v>
+      </c>
+      <c r="AA41" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L42" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N42" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P42" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R42" s="5">
+        <v>0</v>
+      </c>
+      <c r="S42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T42" s="5">
+        <v>0</v>
+      </c>
+      <c r="U42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V42" s="5">
+        <v>0</v>
+      </c>
+      <c r="W42" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L43" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N43" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P43" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R43" s="5">
+        <v>0</v>
+      </c>
+      <c r="S43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T43" s="5">
+        <v>0</v>
+      </c>
+      <c r="U43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V43" s="5">
+        <v>0</v>
+      </c>
+      <c r="W43" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J44" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L44" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N44" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P44" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R44" s="5">
+        <v>0</v>
+      </c>
+      <c r="S44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T44" s="5">
+        <v>0</v>
+      </c>
+      <c r="U44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V44" s="5">
+        <v>0</v>
+      </c>
+      <c r="W44" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J45" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L45" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N45" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P45" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R45" s="5">
+        <v>0</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T45" s="5">
+        <v>0</v>
+      </c>
+      <c r="U45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V45" s="5">
+        <v>0</v>
+      </c>
+      <c r="W45" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J46" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L46" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N46" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P46" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="Q46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R46" s="5">
+        <v>0</v>
+      </c>
+      <c r="S46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T46" s="5">
+        <v>0</v>
+      </c>
+      <c r="U46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V46" s="5">
+        <v>0</v>
+      </c>
+      <c r="W46" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X46" s="5">
+        <v>19</v>
+      </c>
+      <c r="Y46" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J47" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L47" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N47" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="O47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P47" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="Q47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R47" s="5">
+        <v>0</v>
+      </c>
+      <c r="S47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T47" s="5">
+        <v>0</v>
+      </c>
+      <c r="U47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V47" s="5">
+        <v>0</v>
+      </c>
+      <c r="W47" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X47" s="5">
+        <v>46</v>
+      </c>
+      <c r="Y47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J48" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L48" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="M48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N48" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="O48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P48" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="Q48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R48" s="5">
+        <v>0</v>
+      </c>
+      <c r="S48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T48" s="5">
+        <v>0</v>
+      </c>
+      <c r="U48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V48" s="5">
+        <v>0</v>
+      </c>
+      <c r="W48" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X48" s="5">
+        <v>47</v>
+      </c>
+      <c r="Y48" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J49" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L49" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N49" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="O49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P49" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="Q49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R49" s="5">
+        <v>0</v>
+      </c>
+      <c r="S49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T49" s="5">
+        <v>0</v>
+      </c>
+      <c r="U49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V49" s="5">
+        <v>0</v>
+      </c>
+      <c r="W49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X49" s="5">
+        <v>48</v>
+      </c>
+      <c r="Y49" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J50" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L50" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N50" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P50" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R50" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T50" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V50" s="6">
+        <v>0</v>
+      </c>
+      <c r="W50" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X50" s="6">
+        <v>26</v>
+      </c>
+      <c r="Y50" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z50" s="6"/>
+      <c r="AA50" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J51" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L51" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N51" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P51" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R51" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T51" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V51" s="6">
+        <v>0</v>
+      </c>
+      <c r="W51" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X51" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y51" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z51" s="6"/>
+      <c r="AA51" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J52" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L52" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N52" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P52" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R52" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T52" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V52" s="6">
+        <v>0</v>
+      </c>
+      <c r="W52" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X52" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y52" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z52" s="6"/>
+      <c r="AA52" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J53" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L53" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="M53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N53" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P53" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="Q53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R53" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T53" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V53" s="6">
+        <v>7</v>
+      </c>
+      <c r="W53" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X53" s="6"/>
+      <c r="Y53" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z53" s="6"/>
+      <c r="AA53" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J54" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L54" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N54" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P54" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R54" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T54" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V54" s="4">
+        <v>0</v>
+      </c>
+      <c r="W54" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J55" s="4">
+        <v>-0.05</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L55" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N55" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="O55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P55" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="Q55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R55" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="S55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T55" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="U55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V55" s="4">
+        <v>0</v>
+      </c>
+      <c r="W55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z55" s="4"/>
+      <c r="AA55" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J56" s="4">
+        <v>-0.05</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L56" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N56" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P56" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="Q56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R56" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="S56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T56" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="U56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V56" s="4">
+        <v>0</v>
+      </c>
+      <c r="W56" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z56" s="4"/>
+      <c r="AA56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J57" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L57" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N57" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P57" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R57" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T57" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V57" s="4">
+        <v>0</v>
+      </c>
+      <c r="W57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB57" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Fine tuning of some news
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -975,25 +975,25 @@
         <v>35</v>
       </c>
       <c r="J2" s="4">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>35</v>
       </c>
       <c r="L2" s="4">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>35</v>
       </c>
       <c r="N2" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="4">
         <v>0.1</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="4">
-        <v>0.2</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>35</v>
@@ -1057,25 +1057,25 @@
         <v>35</v>
       </c>
       <c r="J3" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="6">
         <v>0.1</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0.2</v>
-      </c>
       <c r="M3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="N3" s="6">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="P3" s="6">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>35</v>
@@ -1175,7 +1175,7 @@
         <v>35</v>
       </c>
       <c r="V4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>80</v>
@@ -5327,7 +5327,7 @@
         <v>35</v>
       </c>
       <c r="V54" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="W54" s="4" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
* Updated formulas and news
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2994,7 +2994,9 @@
       <c r="W26" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="X26" s="6"/>
+      <c r="X26" s="6">
+        <v>24</v>
+      </c>
       <c r="Y26" s="4" t="s">
         <v>81</v>
       </c>
@@ -3076,7 +3078,9 @@
       <c r="W27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="X27" s="6"/>
+      <c r="X27" s="6">
+        <v>25</v>
+      </c>
       <c r="Y27" s="4" t="s">
         <v>81</v>
       </c>
@@ -3158,7 +3162,9 @@
       <c r="W28" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="X28" s="4"/>
+      <c r="X28" s="4">
+        <v>25</v>
+      </c>
       <c r="Y28" s="4" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
* Updated formulas & news
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -402,9 +402,6 @@
     <t>26,49</t>
   </si>
   <si>
-    <t>"Se clausuran las sesiones del congreso a la fuerza, Pajaronia acongojada."</t>
-  </si>
-  <si>
     <t>"Dictador clausura el congreso"</t>
   </si>
   <si>
@@ -430,6 +427,9 @@
   </si>
   <si>
     <t>"El presidente Albatros propone una nueva bandera para Pajaronia. Es un hermoso diseño."</t>
+  </si>
+  <si>
+    <t>"En ataque contra la democracia, se clausuran las sesiones del congreso a la fuerza. Pajaronia acongojada."</t>
   </si>
 </sst>
 </file>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
-      <selection activeCell="X38" sqref="X38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5197,13 +5197,13 @@
         <v>35</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>35</v>
@@ -5279,13 +5279,13 @@
         <v>35</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>35</v>
@@ -5361,13 +5361,13 @@
         <v>35</v>
       </c>
       <c r="D55" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>35</v>
@@ -5443,13 +5443,13 @@
         <v>35</v>
       </c>
       <c r="D56" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>35</v>
@@ -5525,13 +5525,13 @@
         <v>35</v>
       </c>
       <c r="D57" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
* New News * New Balance
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="186">
   <si>
     <t>"Paro de gallos madrugadores"</t>
   </si>
@@ -430,6 +430,150 @@
   </si>
   <si>
     <t>"En ataque contra la democracia, se clausuran las sesiones del congreso a la fuerza. Pajaronia acongojada."</t>
+  </si>
+  <si>
+    <t>"Clausura del Congreso de alta gravedad"</t>
+  </si>
+  <si>
+    <t>"Lo que el país necesita"</t>
+  </si>
+  <si>
+    <t>"Intelectuales del Instituto Pelícano sostienen que la clausura del Congreso es lo que el país necesita para salir adelante"</t>
+  </si>
+  <si>
+    <t>"Constitucionalista Cormorán Gutiérrez sostiene que la clausura del congreso afecta seriamente las chances de la vuelta de la democracia"</t>
+  </si>
+  <si>
+    <t>"Flamencos manifiestan preocupación frente al avance ante derechos civiles."</t>
+  </si>
+  <si>
+    <t>"Cuervos en éxtasis ante posibilidad de nuevos negocios con el gobierno, sostienen que crecerá el empleo."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Flamencos preocupados"</t>
+  </si>
+  <si>
+    <t>"Cuervos extasiados"</t>
+  </si>
+  <si>
+    <t>"Alpiste para tod@s"</t>
+  </si>
+  <si>
+    <t>"Notebooks para tod@s"</t>
+  </si>
+  <si>
+    <t>"Planes para tod@s"</t>
+  </si>
+  <si>
+    <t>"Dolares para tod@s"</t>
+  </si>
+  <si>
+    <t>"Se podran obtener dolares en los bebederos y fuentes de la nación."</t>
+  </si>
+  <si>
+    <t>"La esposa del presidente da a conocer su nueva línea de perfumes."</t>
+  </si>
+  <si>
+    <t>"Le Prefum"</t>
+  </si>
+  <si>
+    <t>"Cacona Voladora"</t>
+  </si>
+  <si>
+    <t>"Se levanto el toque de queda para mover el intestino mientras se vuela."</t>
+  </si>
+  <si>
+    <t>"Cacona Generadora"</t>
+  </si>
+  <si>
+    <t>"Se contratan 200 empleados para limpiar la cacona venidera"</t>
+  </si>
+  <si>
+    <t>"Nuevos parajes"</t>
+  </si>
+  <si>
+    <t>"La isla de los murcielagos abre sus puertas."</t>
+  </si>
+  <si>
+    <t>"Sale y vale"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Se cierra trato con Mucielandia para visitas guiadas durante el día, el presidente afirma que todos nos beneficiaremos de este acuerdo"</t>
+  </si>
+  <si>
+    <t>"Mar del Cobre"</t>
+  </si>
+  <si>
+    <t>"Marcha de pavos reales"</t>
+  </si>
+  <si>
+    <t>"Muestran orgullosamente sus plumas durante este fin de semana."</t>
+  </si>
+  <si>
+    <t>"El teatro de revistas en su auge, los turistas invaden las playas."</t>
+  </si>
+  <si>
+    <t>"Los esperados colibríes"</t>
+  </si>
+  <si>
+    <t>"Los hermosos Colibríes realizaran su tan ansiado baile anual en la plaza San Cotorra"</t>
+  </si>
+  <si>
+    <t>"Carnaval Carioca"</t>
+  </si>
+  <si>
+    <t>"Como todos los años se festejara el carnaval en el sambodromo del Avestruz atrevido."</t>
+  </si>
+  <si>
+    <t>"Inversiones"</t>
+  </si>
+  <si>
+    <t>"El gobierno invierte en investigación aviar."</t>
+  </si>
+  <si>
+    <t>"Júbilo para los jubilados"</t>
+  </si>
+  <si>
+    <t>"Se aumentara la jubilación, abuelos felices."</t>
+  </si>
+  <si>
+    <t>"Apoyo de los Estados Halconísticos"</t>
+  </si>
+  <si>
+    <t>"El nuevo gabinete estará conformado por diferentes amigos del nuevo Presidente."</t>
+  </si>
+  <si>
+    <t>"Confirma el Presidente el nuevo gabinete"</t>
+  </si>
+  <si>
+    <t>"Tensión en la Región"</t>
+  </si>
+  <si>
+    <t>"Los vecinos países del Aladosur, se mantienen en alerta tras el golpe de estado del General Albatros."</t>
+  </si>
+  <si>
+    <t>"El embajador Hawkins de los EEHH manifestó su apoyo al General Albatros. Es lo que Pajaronia necesita, manifestó."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Estado de Sitio"</t>
+  </si>
+  <si>
+    <t>"El Gobierno decretó el estado de sitio, con toque de queda desde las 9PM hasta las 5AM."</t>
+  </si>
+  <si>
+    <t>"Ajusticiamiento"</t>
+  </si>
+  <si>
+    <t>"Rumores indicarían que tropas afines al gobierno habrían ajusticiado a diferentes opositores."</t>
+  </si>
+  <si>
+    <t>"El nuevo gobierno entrega alpiste y elementos de la canaste familiar a las familias mas necesitadas."</t>
+  </si>
+  <si>
+    <t>"El nuevo gobierno entrega notebooks a los pichones para acelerar su educación."</t>
+  </si>
+  <si>
+    <t>"El nuevo gobierno entregara planes familiares de vivienda a las familias mas carenciadas."</t>
   </si>
 </sst>
 </file>
@@ -439,7 +583,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +615,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,7 +671,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -532,6 +682,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -837,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB57"/>
+  <dimension ref="A1:AB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3487,7 +3640,7 @@
         <v>35</v>
       </c>
       <c r="V32" s="6">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="W32" s="6" t="s">
         <v>80</v>
@@ -5251,7 +5404,7 @@
         <v>35</v>
       </c>
       <c r="V53" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="W53" s="6" t="s">
         <v>80</v>
@@ -5333,7 +5486,7 @@
         <v>35</v>
       </c>
       <c r="V54" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="W54" s="4" t="s">
         <v>80</v>
@@ -5593,6 +5746,1982 @@
         <v>82</v>
       </c>
       <c r="AB57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J58" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L58" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N58" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P58" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R58" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T58" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V58" s="6">
+        <v>0</v>
+      </c>
+      <c r="W58" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X58" s="6">
+        <v>52</v>
+      </c>
+      <c r="Y58" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z58" s="6"/>
+      <c r="AA58" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J59" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L59" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N59" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P59" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R59" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T59" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V59" s="4">
+        <v>0</v>
+      </c>
+      <c r="W59" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X59" s="4"/>
+      <c r="Y59" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z59" s="4"/>
+      <c r="AA59" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J60" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L60" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N60" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P60" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R60" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T60" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V60" s="6">
+        <v>0</v>
+      </c>
+      <c r="W60" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X60" s="6"/>
+      <c r="Y60" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z60" s="6"/>
+      <c r="AA60" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>36</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J61" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L61" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N61" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P61" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R61" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T61" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V61" s="4">
+        <v>0</v>
+      </c>
+      <c r="W61" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X61" s="4"/>
+      <c r="Y61" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z61" s="4"/>
+      <c r="AA61" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>36</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J62" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L62" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N62" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P62" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R62" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T62" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V62" s="4">
+        <v>0</v>
+      </c>
+      <c r="W62" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X62" s="4"/>
+      <c r="Y62" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z62" s="4"/>
+      <c r="AA62" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J63" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L63" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N63" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P63" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R63" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T63" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V63" s="4">
+        <v>0</v>
+      </c>
+      <c r="W63" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X63" s="4"/>
+      <c r="Y63" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z63" s="4"/>
+      <c r="AA63" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J64" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L64" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N64" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R64" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T64" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V64" s="4">
+        <v>0</v>
+      </c>
+      <c r="W64" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X64" s="4"/>
+      <c r="Y64" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z64" s="4"/>
+      <c r="AA64" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J65" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L65" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N65" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P65" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R65" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T65" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V65" s="4">
+        <v>0</v>
+      </c>
+      <c r="W65" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X65" s="4"/>
+      <c r="Y65" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z65" s="4"/>
+      <c r="AA65" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L66" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N66" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P66" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R66" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T66" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V66" s="4">
+        <v>0</v>
+      </c>
+      <c r="W66" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X66" s="4"/>
+      <c r="Y66" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z66" s="4"/>
+      <c r="AA66" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L67" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N67" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P67" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R67" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T67" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V67" s="4">
+        <v>0</v>
+      </c>
+      <c r="W67" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X67" s="4"/>
+      <c r="Y67" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z67" s="4"/>
+      <c r="AA67" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J68" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L68" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N68" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P68" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R68" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T68" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V68" s="4">
+        <v>0</v>
+      </c>
+      <c r="W68" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X68" s="4">
+        <v>66</v>
+      </c>
+      <c r="Y68" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z68" s="4"/>
+      <c r="AA68" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>36</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J69" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L69" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N69" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P69" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R69" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T69" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V69" s="4">
+        <v>0</v>
+      </c>
+      <c r="W69" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X69" s="4"/>
+      <c r="Y69" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z69" s="4"/>
+      <c r="AA69" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J70" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L70" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N70" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P70" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R70" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T70" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V70" s="4">
+        <v>0</v>
+      </c>
+      <c r="W70" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X70" s="4">
+        <v>68</v>
+      </c>
+      <c r="Y70" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z70" s="4"/>
+      <c r="AA70" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J71" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L71" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N71" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P71" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R71" s="5">
+        <v>0</v>
+      </c>
+      <c r="S71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T71" s="5">
+        <v>0</v>
+      </c>
+      <c r="U71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V71" s="5">
+        <v>0</v>
+      </c>
+      <c r="W71" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X71" s="5"/>
+      <c r="Y71" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z71" s="5"/>
+      <c r="AA71" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J72" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L72" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N72" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P72" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R72" s="5">
+        <v>0</v>
+      </c>
+      <c r="S72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T72" s="5">
+        <v>0</v>
+      </c>
+      <c r="U72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V72" s="5">
+        <v>0</v>
+      </c>
+      <c r="W72" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X72" s="5"/>
+      <c r="Y72" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z72" s="5"/>
+      <c r="AA72" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J73" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L73" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N73" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P73" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R73" s="5">
+        <v>0</v>
+      </c>
+      <c r="S73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T73" s="5">
+        <v>0</v>
+      </c>
+      <c r="U73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V73" s="5">
+        <v>0</v>
+      </c>
+      <c r="W73" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X73" s="5"/>
+      <c r="Y73" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z73" s="5"/>
+      <c r="AA73" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L74" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N74" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P74" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R74" s="5">
+        <v>0</v>
+      </c>
+      <c r="S74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T74" s="5">
+        <v>0</v>
+      </c>
+      <c r="U74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V74" s="5">
+        <v>0</v>
+      </c>
+      <c r="W74" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X74" s="5"/>
+      <c r="Y74" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z74" s="5"/>
+      <c r="AA74" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J75" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L75" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N75" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P75" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R75" s="5">
+        <v>0</v>
+      </c>
+      <c r="S75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T75" s="5">
+        <v>0</v>
+      </c>
+      <c r="U75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V75" s="5">
+        <v>0</v>
+      </c>
+      <c r="W75" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X75" s="5"/>
+      <c r="Y75" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z75" s="5"/>
+      <c r="AA75" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J76" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L76" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N76" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="O76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P76" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="Q76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R76" s="5">
+        <v>0</v>
+      </c>
+      <c r="S76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T76" s="5">
+        <v>0</v>
+      </c>
+      <c r="U76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V76" s="5">
+        <v>0</v>
+      </c>
+      <c r="W76" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="X76" s="5"/>
+      <c r="Y76" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z76" s="5"/>
+      <c r="AA76" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J77" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L77" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N77" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P77" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R77" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T77" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V77" s="4">
+        <v>0</v>
+      </c>
+      <c r="W77" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X77" s="4">
+        <v>77</v>
+      </c>
+      <c r="Y77" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z77" s="4"/>
+      <c r="AA77" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>36</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J78" s="4">
+        <v>-0.04</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L78" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N78" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="O78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P78" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="Q78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R78" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T78" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="U78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V78" s="4">
+        <v>0</v>
+      </c>
+      <c r="W78" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X78" s="4"/>
+      <c r="Y78" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z78" s="4"/>
+      <c r="AA78" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F79" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H79" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I79" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J79" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="K79" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L79" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="M79" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N79" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="O79" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P79" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="Q79" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R79" s="7">
+        <v>-0.05</v>
+      </c>
+      <c r="S79" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="T79" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="U79" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="V79" s="9">
+        <v>0</v>
+      </c>
+      <c r="W79" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="X79" s="9"/>
+      <c r="Y79" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z79" s="9"/>
+      <c r="AA79" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>36</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G80" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H80" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J80" s="12">
+        <v>-0.01</v>
+      </c>
+      <c r="K80" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L80" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="M80" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N80" s="12">
+        <v>-0.01</v>
+      </c>
+      <c r="O80" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P80" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q80" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R80" s="7">
+        <v>-0.1</v>
+      </c>
+      <c r="S80" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="T80" s="7">
+        <v>0</v>
+      </c>
+      <c r="U80" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="V80" s="9">
+        <v>10</v>
+      </c>
+      <c r="W80" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="X80" s="9"/>
+      <c r="Y80" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z80" s="9"/>
+      <c r="AA80" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J81" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L81" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N81" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P81" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R81" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="S81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T81" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V81" s="6">
+        <v>0</v>
+      </c>
+      <c r="W81" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X81" s="6"/>
+      <c r="Y81" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z81" s="6"/>
+      <c r="AA81" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB81" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Updated News & Scene
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -372,9 +372,6 @@
     <t>"Hace rato que nadie le arrastra el ala a la Urraca, sostiene desde el estudio."</t>
   </si>
   <si>
-    <t>"Divas y algo más"</t>
-  </si>
-  <si>
     <t>"Avistaron a La Garza Giménes y a la Urraca Casandra a los besos en la playa del Pato Lucas,  estaban mas calientes que la arena dijo una Paloma que pasaba."</t>
   </si>
   <si>
@@ -574,6 +571,9 @@
   </si>
   <si>
     <t>"El nuevo gobierno entregara planes familiares de vivienda a las familias mas carenciadas."</t>
+  </si>
+  <si>
+    <t>"PRIMICIA: Divas y algo más"</t>
   </si>
 </sst>
 </file>
@@ -992,9 +992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1298,7 +1296,7 @@
         <v>35</v>
       </c>
       <c r="L4" s="5">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>35</v>
@@ -1310,7 +1308,7 @@
         <v>35</v>
       </c>
       <c r="P4" s="5">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>35</v>
@@ -1626,7 +1624,7 @@
         <v>35</v>
       </c>
       <c r="L8" s="5">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>35</v>
@@ -1638,7 +1636,7 @@
         <v>35</v>
       </c>
       <c r="P8" s="5">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>35</v>
@@ -1708,7 +1706,7 @@
         <v>35</v>
       </c>
       <c r="L9" s="5">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>35</v>
@@ -1720,7 +1718,7 @@
         <v>35</v>
       </c>
       <c r="P9" s="5">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="Q9" s="5" t="s">
         <v>35</v>
@@ -1790,7 +1788,7 @@
         <v>35</v>
       </c>
       <c r="L10" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>35</v>
@@ -1802,7 +1800,7 @@
         <v>35</v>
       </c>
       <c r="P10" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q10" s="5" t="s">
         <v>35</v>
@@ -2126,7 +2124,7 @@
         <v>35</v>
       </c>
       <c r="L14" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>35</v>
@@ -2138,7 +2136,7 @@
         <v>35</v>
       </c>
       <c r="P14" s="5">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="Q14" s="5" t="s">
         <v>35</v>
@@ -2290,7 +2288,7 @@
         <v>35</v>
       </c>
       <c r="L16" s="5">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>35</v>
@@ -2302,7 +2300,7 @@
         <v>35</v>
       </c>
       <c r="P16" s="5">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="Q16" s="5" t="s">
         <v>35</v>
@@ -2372,7 +2370,7 @@
         <v>35</v>
       </c>
       <c r="L17" s="5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>35</v>
@@ -2384,7 +2382,7 @@
         <v>35</v>
       </c>
       <c r="P17" s="5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="Q17" s="5" t="s">
         <v>35</v>
@@ -2618,7 +2616,7 @@
         <v>35</v>
       </c>
       <c r="L20" s="5">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>35</v>
@@ -2630,7 +2628,7 @@
         <v>35</v>
       </c>
       <c r="P20" s="5">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>35</v>
@@ -2776,25 +2774,25 @@
         <v>35</v>
       </c>
       <c r="J22" s="5">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L22" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" s="5">
         <v>-0.02</v>
       </c>
-      <c r="M22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="5">
-        <v>-0.03</v>
-      </c>
       <c r="O22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P22" s="5">
-        <v>-0.02</v>
+        <v>0.02</v>
       </c>
       <c r="Q22" s="5" t="s">
         <v>35</v>
@@ -2864,7 +2862,7 @@
         <v>35</v>
       </c>
       <c r="L23" s="5">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>35</v>
@@ -2876,7 +2874,7 @@
         <v>35</v>
       </c>
       <c r="P23" s="5">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="Q23" s="5" t="s">
         <v>35</v>
@@ -2948,7 +2946,7 @@
         <v>35</v>
       </c>
       <c r="L24" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>35</v>
@@ -2960,7 +2958,7 @@
         <v>35</v>
       </c>
       <c r="P24" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q24" s="5" t="s">
         <v>35</v>
@@ -3364,7 +3362,7 @@
         <v>35</v>
       </c>
       <c r="L29" s="5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="M29" s="5" t="s">
         <v>35</v>
@@ -3376,7 +3374,7 @@
         <v>35</v>
       </c>
       <c r="P29" s="5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="Q29" s="5" t="s">
         <v>35</v>
@@ -3640,7 +3638,7 @@
         <v>35</v>
       </c>
       <c r="V32" s="6">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="W32" s="6" t="s">
         <v>80</v>
@@ -3950,7 +3948,7 @@
         <v>35</v>
       </c>
       <c r="L36" s="5">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="M36" s="5" t="s">
         <v>35</v>
@@ -3962,7 +3960,7 @@
         <v>35</v>
       </c>
       <c r="P36" s="5">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="Q36" s="5" t="s">
         <v>35</v>
@@ -4036,7 +4034,7 @@
         <v>35</v>
       </c>
       <c r="L37" s="5">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>35</v>
@@ -4048,7 +4046,7 @@
         <v>35</v>
       </c>
       <c r="P37" s="5">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="Q37" s="5" t="s">
         <v>35</v>
@@ -4122,7 +4120,7 @@
         <v>35</v>
       </c>
       <c r="L38" s="5">
-        <v>-0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>35</v>
@@ -4134,7 +4132,7 @@
         <v>35</v>
       </c>
       <c r="P38" s="5">
-        <v>-0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q38" s="5" t="s">
         <v>35</v>
@@ -4206,7 +4204,7 @@
         <v>35</v>
       </c>
       <c r="L39" s="5">
-        <v>-0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>35</v>
@@ -4218,7 +4216,7 @@
         <v>35</v>
       </c>
       <c r="P39" s="5">
-        <v>-0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q39" s="5" t="s">
         <v>35</v>
@@ -4290,7 +4288,7 @@
         <v>35</v>
       </c>
       <c r="L40" s="5">
-        <v>-0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>35</v>
@@ -4302,7 +4300,7 @@
         <v>35</v>
       </c>
       <c r="P40" s="5">
-        <v>-0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q40" s="5" t="s">
         <v>35</v>
@@ -4374,7 +4372,7 @@
         <v>35</v>
       </c>
       <c r="L41" s="5">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>35</v>
@@ -4386,7 +4384,7 @@
         <v>35</v>
       </c>
       <c r="P41" s="5">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="Q41" s="5" t="s">
         <v>35</v>
@@ -4452,25 +4450,25 @@
         <v>35</v>
       </c>
       <c r="J42" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L42" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N42" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="O42" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P42" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q42" s="5" t="s">
         <v>35</v>
@@ -4534,25 +4532,25 @@
         <v>35</v>
       </c>
       <c r="J43" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L43" s="5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N43" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="O43" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P43" s="5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="Q43" s="5" t="s">
         <v>35</v>
@@ -4616,25 +4614,25 @@
         <v>35</v>
       </c>
       <c r="J44" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L44" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M44" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N44" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="O44" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P44" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q44" s="5" t="s">
         <v>35</v>
@@ -4698,25 +4696,25 @@
         <v>35</v>
       </c>
       <c r="J45" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L45" s="5">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="M45" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N45" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="O45" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P45" s="5">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="Q45" s="5" t="s">
         <v>35</v>
@@ -4780,25 +4778,25 @@
         <v>35</v>
       </c>
       <c r="J46" s="5">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L46" s="5">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="M46" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N46" s="5">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="O46" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P46" s="5">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="Q46" s="5" t="s">
         <v>35</v>
@@ -4864,25 +4862,25 @@
         <v>35</v>
       </c>
       <c r="J47" s="5">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L47" s="5">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="M47" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N47" s="5">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="O47" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P47" s="5">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="Q47" s="5" t="s">
         <v>35</v>
@@ -4948,25 +4946,25 @@
         <v>35</v>
       </c>
       <c r="J48" s="5">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L48" s="5">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="M48" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N48" s="5">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="O48" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P48" s="5">
-        <v>-0.01</v>
+        <v>0.05</v>
       </c>
       <c r="Q48" s="5" t="s">
         <v>35</v>
@@ -5014,14 +5012,14 @@
         <v>35</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="G49" s="5" t="s">
         <v>35</v>
       </c>
@@ -5032,25 +5030,25 @@
         <v>35</v>
       </c>
       <c r="J49" s="5">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L49" s="5">
-        <v>-0.01</v>
+        <v>0.1</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N49" s="5">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="O49" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P49" s="5">
-        <v>-0.01</v>
+        <v>0.1</v>
       </c>
       <c r="Q49" s="5" t="s">
         <v>35</v>
@@ -5098,13 +5096,13 @@
         <v>35</v>
       </c>
       <c r="D50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>35</v>
@@ -5182,13 +5180,13 @@
         <v>35</v>
       </c>
       <c r="D51" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>35</v>
@@ -5242,7 +5240,7 @@
         <v>80</v>
       </c>
       <c r="X51" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y51" s="6" t="s">
         <v>81</v>
@@ -5266,13 +5264,13 @@
         <v>35</v>
       </c>
       <c r="D52" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>35</v>
@@ -5326,7 +5324,7 @@
         <v>80</v>
       </c>
       <c r="X52" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Y52" s="6" t="s">
         <v>81</v>
@@ -5350,13 +5348,13 @@
         <v>35</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>35</v>
@@ -5404,7 +5402,7 @@
         <v>35</v>
       </c>
       <c r="V53" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W53" s="6" t="s">
         <v>80</v>
@@ -5432,13 +5430,13 @@
         <v>35</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>35</v>
@@ -5486,7 +5484,7 @@
         <v>35</v>
       </c>
       <c r="V54" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W54" s="4" t="s">
         <v>80</v>
@@ -5514,13 +5512,13 @@
         <v>35</v>
       </c>
       <c r="D55" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>35</v>
@@ -5596,13 +5594,13 @@
         <v>35</v>
       </c>
       <c r="D56" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>35</v>
@@ -5678,13 +5676,13 @@
         <v>35</v>
       </c>
       <c r="D57" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>35</v>
@@ -5760,13 +5758,13 @@
         <v>35</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>35</v>
@@ -5844,13 +5842,13 @@
         <v>35</v>
       </c>
       <c r="D59" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>35</v>
@@ -5926,13 +5924,13 @@
         <v>35</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>35</v>
@@ -6008,13 +6006,13 @@
         <v>35</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>35</v>
@@ -6090,13 +6088,13 @@
         <v>35</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>35</v>
@@ -6172,13 +6170,13 @@
         <v>35</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>35</v>
@@ -6254,13 +6252,13 @@
         <v>35</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>35</v>
@@ -6336,13 +6334,13 @@
         <v>35</v>
       </c>
       <c r="D65" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F65" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>35</v>
@@ -6418,13 +6416,13 @@
         <v>35</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>35</v>
@@ -6500,13 +6498,13 @@
         <v>35</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F67" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>35</v>
@@ -6582,13 +6580,13 @@
         <v>35</v>
       </c>
       <c r="D68" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>35</v>
@@ -6666,13 +6664,13 @@
         <v>35</v>
       </c>
       <c r="D69" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F69" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>35</v>
@@ -6748,13 +6746,13 @@
         <v>35</v>
       </c>
       <c r="D70" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F70" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>35</v>
@@ -6832,13 +6830,13 @@
         <v>35</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>35</v>
@@ -6856,7 +6854,7 @@
         <v>35</v>
       </c>
       <c r="L71" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M71" s="5" t="s">
         <v>35</v>
@@ -6868,7 +6866,7 @@
         <v>35</v>
       </c>
       <c r="P71" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q71" s="5" t="s">
         <v>35</v>
@@ -6914,13 +6912,13 @@
         <v>35</v>
       </c>
       <c r="D72" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F72" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>35</v>
@@ -6938,7 +6936,7 @@
         <v>35</v>
       </c>
       <c r="L72" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M72" s="5" t="s">
         <v>35</v>
@@ -6950,7 +6948,7 @@
         <v>35</v>
       </c>
       <c r="P72" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q72" s="5" t="s">
         <v>35</v>
@@ -6996,13 +6994,13 @@
         <v>35</v>
       </c>
       <c r="D73" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F73" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>35</v>
@@ -7020,7 +7018,7 @@
         <v>35</v>
       </c>
       <c r="L73" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M73" s="5" t="s">
         <v>35</v>
@@ -7032,7 +7030,7 @@
         <v>35</v>
       </c>
       <c r="P73" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q73" s="5" t="s">
         <v>35</v>
@@ -7078,13 +7076,13 @@
         <v>35</v>
       </c>
       <c r="D74" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F74" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>35</v>
@@ -7102,7 +7100,7 @@
         <v>35</v>
       </c>
       <c r="L74" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M74" s="5" t="s">
         <v>35</v>
@@ -7114,7 +7112,7 @@
         <v>35</v>
       </c>
       <c r="P74" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q74" s="5" t="s">
         <v>35</v>
@@ -7160,14 +7158,14 @@
         <v>35</v>
       </c>
       <c r="D75" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F75" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E75" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>170</v>
-      </c>
       <c r="G75" s="5" t="s">
         <v>35</v>
       </c>
@@ -7178,25 +7176,25 @@
         <v>35</v>
       </c>
       <c r="J75" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="K75" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L75" s="5">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="M75" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N75" s="5">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="O75" s="5" t="s">
         <v>35</v>
       </c>
       <c r="P75" s="5">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="Q75" s="5" t="s">
         <v>35</v>
@@ -7242,13 +7240,13 @@
         <v>35</v>
       </c>
       <c r="D76" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>172</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>35</v>
@@ -7266,7 +7264,7 @@
         <v>35</v>
       </c>
       <c r="L76" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M76" s="5" t="s">
         <v>35</v>
@@ -7278,7 +7276,7 @@
         <v>35</v>
       </c>
       <c r="P76" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="Q76" s="5" t="s">
         <v>35</v>
@@ -7324,13 +7322,13 @@
         <v>35</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>35</v>
@@ -7408,13 +7406,13 @@
         <v>35</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>35</v>
@@ -7490,13 +7488,13 @@
         <v>35</v>
       </c>
       <c r="D79" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F79" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="E79" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F79" s="12" t="s">
-        <v>177</v>
       </c>
       <c r="G79" s="11" t="s">
         <v>35</v>
@@ -7572,13 +7570,13 @@
         <v>35</v>
       </c>
       <c r="D80" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>35</v>
@@ -7626,7 +7624,7 @@
         <v>35</v>
       </c>
       <c r="V80" s="9">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="W80" s="9" t="s">
         <v>80</v>
@@ -7654,13 +7652,13 @@
         <v>35</v>
       </c>
       <c r="D81" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F81" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
* Added endgame texts * Added debug stats
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="196">
   <si>
     <t>"Paro de gallos madrugadores"</t>
   </si>
@@ -574,6 +574,36 @@
   </si>
   <si>
     <t>"PRIMICIA: Divas y algo más"</t>
+  </si>
+  <si>
+    <t>"ExPresidente Palometa, exiliado en Murcielandia"</t>
+  </si>
+  <si>
+    <t>"El ExPresidente fue recibido por autoridades de Murcielandia, en donde se encuentra exiliado."</t>
+  </si>
+  <si>
+    <t>"Devastadoras declaraciones de ExPresidente Palometa"</t>
+  </si>
+  <si>
+    <t>"Dijo: Me taparon los ojos, y me obligaron a dejar el palacio presidencial. Es un golpe de lo mas ruin."</t>
+  </si>
+  <si>
+    <t>"ExPresidente Palometa se ha suicidado"</t>
+  </si>
+  <si>
+    <t>"Fue encontrado en dudosas circunstancias. El peritaje inicial no es concluyente."</t>
+  </si>
+  <si>
+    <t>"Autopsia de Palometa"</t>
+  </si>
+  <si>
+    <t>"Los resultados indican que se trataría de un magnicidio, servicios de inteligencia de Albatros, sospechados."</t>
+  </si>
+  <si>
+    <t>"La autopsia de Palometa es un circo"</t>
+  </si>
+  <si>
+    <t>"Expertos internacionales indican que la autopsia es un circo, que indiscutiblemente fue suicidio por la situación en la que dejó el país."</t>
   </si>
 </sst>
 </file>
@@ -990,9 +1020,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB81"/>
+  <dimension ref="A1:AB86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1150,13 +1182,13 @@
         <v>35</v>
       </c>
       <c r="R2" s="4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T2" s="4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>35</v>
@@ -1232,13 +1264,13 @@
         <v>35</v>
       </c>
       <c r="R3" s="6">
-        <v>0</v>
+        <v>-0.06</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="T3" s="6">
-        <v>0</v>
+        <v>-0.03</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>35</v>
@@ -1396,7 +1428,7 @@
         <v>35</v>
       </c>
       <c r="R5" s="6">
-        <v>-0.03</v>
+        <v>-0.06</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>35</v>
@@ -1478,7 +1510,7 @@
         <v>35</v>
       </c>
       <c r="R6" s="6">
-        <v>-0.02</v>
+        <v>-0.06</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>35</v>
@@ -1560,7 +1592,7 @@
         <v>35</v>
       </c>
       <c r="R7" s="6">
-        <v>-0.02</v>
+        <v>-0.04</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>35</v>
@@ -1888,13 +1920,13 @@
         <v>35</v>
       </c>
       <c r="R11" s="6">
-        <v>-0.03</v>
+        <v>-0.1</v>
       </c>
       <c r="S11" s="6" t="s">
         <v>35</v>
       </c>
       <c r="T11" s="6">
-        <v>-0.01</v>
+        <v>-0.05</v>
       </c>
       <c r="U11" s="6" t="s">
         <v>35</v>
@@ -2722,7 +2754,7 @@
         <v>35</v>
       </c>
       <c r="T21" s="6">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="U21" s="6" t="s">
         <v>35</v>
@@ -3046,7 +3078,7 @@
         <v>35</v>
       </c>
       <c r="R25" s="6">
-        <v>-0.02</v>
+        <v>-0.05</v>
       </c>
       <c r="S25" s="6" t="s">
         <v>35</v>
@@ -3128,7 +3160,7 @@
         <v>35</v>
       </c>
       <c r="R26" s="6">
-        <v>-0.02</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="S26" s="6" t="s">
         <v>35</v>
@@ -3212,7 +3244,7 @@
         <v>35</v>
       </c>
       <c r="R27" s="6">
-        <v>-0.04</v>
+        <v>-0.1</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>35</v>
@@ -3550,7 +3582,7 @@
         <v>35</v>
       </c>
       <c r="T31" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U31" s="4" t="s">
         <v>35</v>
@@ -3626,7 +3658,7 @@
         <v>35</v>
       </c>
       <c r="R32" s="6">
-        <v>-0.04</v>
+        <v>-0.1</v>
       </c>
       <c r="S32" s="6" t="s">
         <v>35</v>
@@ -3710,7 +3742,7 @@
         <v>35</v>
       </c>
       <c r="R33" s="6">
-        <v>-0.04</v>
+        <v>-0.1</v>
       </c>
       <c r="S33" s="6" t="s">
         <v>35</v>
@@ -3880,7 +3912,7 @@
         <v>35</v>
       </c>
       <c r="R35" s="4">
-        <v>0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>35</v>
@@ -5138,7 +5170,7 @@
         <v>35</v>
       </c>
       <c r="R50" s="6">
-        <v>-0.04</v>
+        <v>-0.1</v>
       </c>
       <c r="S50" s="6" t="s">
         <v>35</v>
@@ -5222,7 +5254,7 @@
         <v>35</v>
       </c>
       <c r="R51" s="6">
-        <v>-0.04</v>
+        <v>-0.06</v>
       </c>
       <c r="S51" s="6" t="s">
         <v>35</v>
@@ -5306,7 +5338,7 @@
         <v>35</v>
       </c>
       <c r="R52" s="6">
-        <v>-0.04</v>
+        <v>-0.06</v>
       </c>
       <c r="S52" s="6" t="s">
         <v>35</v>
@@ -5390,7 +5422,7 @@
         <v>35</v>
       </c>
       <c r="R53" s="6">
-        <v>-0.04</v>
+        <v>-0.06</v>
       </c>
       <c r="S53" s="6" t="s">
         <v>35</v>
@@ -5472,13 +5504,13 @@
         <v>35</v>
       </c>
       <c r="R54" s="4">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="S54" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T54" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U54" s="4" t="s">
         <v>35</v>
@@ -5724,7 +5756,7 @@
         <v>35</v>
       </c>
       <c r="T57" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U57" s="4" t="s">
         <v>35</v>
@@ -5800,7 +5832,7 @@
         <v>35</v>
       </c>
       <c r="R58" s="6">
-        <v>-0.04</v>
+        <v>-0.06</v>
       </c>
       <c r="S58" s="6" t="s">
         <v>35</v>
@@ -5890,7 +5922,7 @@
         <v>35</v>
       </c>
       <c r="T59" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U59" s="4" t="s">
         <v>35</v>
@@ -5966,7 +5998,7 @@
         <v>35</v>
       </c>
       <c r="R60" s="6">
-        <v>-0.04</v>
+        <v>-0.06</v>
       </c>
       <c r="S60" s="6" t="s">
         <v>35</v>
@@ -6054,7 +6086,7 @@
         <v>35</v>
       </c>
       <c r="T61" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U61" s="4" t="s">
         <v>35</v>
@@ -6136,7 +6168,7 @@
         <v>35</v>
       </c>
       <c r="T62" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U62" s="4" t="s">
         <v>35</v>
@@ -6218,7 +6250,7 @@
         <v>35</v>
       </c>
       <c r="T63" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U63" s="4" t="s">
         <v>35</v>
@@ -6300,7 +6332,7 @@
         <v>35</v>
       </c>
       <c r="T64" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U64" s="4" t="s">
         <v>35</v>
@@ -6382,7 +6414,7 @@
         <v>35</v>
       </c>
       <c r="T65" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U65" s="4" t="s">
         <v>35</v>
@@ -6464,7 +6496,7 @@
         <v>35</v>
       </c>
       <c r="T66" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U66" s="4" t="s">
         <v>35</v>
@@ -6546,7 +6578,7 @@
         <v>35</v>
       </c>
       <c r="T67" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U67" s="4" t="s">
         <v>35</v>
@@ -6628,7 +6660,7 @@
         <v>35</v>
       </c>
       <c r="T68" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U68" s="4" t="s">
         <v>35</v>
@@ -6712,7 +6744,7 @@
         <v>35</v>
       </c>
       <c r="T69" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U69" s="4" t="s">
         <v>35</v>
@@ -6794,7 +6826,7 @@
         <v>35</v>
       </c>
       <c r="T70" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U70" s="4" t="s">
         <v>35</v>
@@ -7370,7 +7402,7 @@
         <v>35</v>
       </c>
       <c r="T77" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U77" s="4" t="s">
         <v>35</v>
@@ -7454,7 +7486,7 @@
         <v>35</v>
       </c>
       <c r="T78" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="U78" s="4" t="s">
         <v>35</v>
@@ -7694,7 +7726,7 @@
         <v>35</v>
       </c>
       <c r="R81" s="6">
-        <v>-0.04</v>
+        <v>-0.1</v>
       </c>
       <c r="S81" s="6" t="s">
         <v>35</v>
@@ -7720,6 +7752,416 @@
         <v>82</v>
       </c>
       <c r="AB81" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>36</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J82" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L82" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N82" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P82" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R82" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="S82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T82" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U82" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V82" s="6">
+        <v>0</v>
+      </c>
+      <c r="W82" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X82" s="6"/>
+      <c r="Y82" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z82" s="6"/>
+      <c r="AA82" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J83" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L83" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N83" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P83" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R83" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="S83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T83" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U83" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V83" s="6">
+        <v>81</v>
+      </c>
+      <c r="W83" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X83" s="6"/>
+      <c r="Y83" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z83" s="6"/>
+      <c r="AA83" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J84" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L84" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N84" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P84" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R84" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="S84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T84" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V84" s="6">
+        <v>82</v>
+      </c>
+      <c r="W84" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X84" s="6"/>
+      <c r="Y84" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z84" s="6"/>
+      <c r="AA84" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>36</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J85" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L85" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="M85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N85" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="O85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P85" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="Q85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R85" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="S85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T85" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="U85" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V85" s="6">
+        <v>83</v>
+      </c>
+      <c r="W85" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X85" s="6"/>
+      <c r="Y85" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z85" s="6"/>
+      <c r="AA85" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>36</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J86" s="4">
+        <v>-0.04</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L86" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N86" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="O86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P86" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="Q86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R86" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T86" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="U86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V86" s="4">
+        <v>83</v>
+      </c>
+      <c r="W86" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X86" s="4"/>
+      <c r="Y86" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z86" s="4"/>
+      <c r="AA86" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB86" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved display of stats in game.
</commit_message>
<xml_diff>
--- a/Documentation/MasterNews.xlsx
+++ b/Documentation/MasterNews.xlsx
@@ -219,9 +219,6 @@
     <t>"Jubilado asalta a efectivos policiales mientras intentaban contener una turba enfurecida."</t>
   </si>
   <si>
-    <t>"La policía actuó rápidamente capturando a un malechor en pleno acto, declaro que fue gracias al gran entrenamiento policial."</t>
-  </si>
-  <si>
     <t>"Mas vale pájaro en mano"</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>"La isla de los murciélagos abre sus puertas."</t>
+  </si>
+  <si>
+    <t>"La policía actuó rápidamente capturando a un malhechor en pleno acto, declaro que fue gracias al gran entrenamiento policial."</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1045,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G71" workbookViewId="0">
+      <selection activeCell="AB81" sqref="AB81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1075,7 +1077,7 @@
         <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
@@ -1093,7 +1095,7 @@
         <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
         <v>32</v>
@@ -1135,19 +1137,19 @@
         <v>32</v>
       </c>
       <c r="V1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W1" t="s">
         <v>32</v>
       </c>
       <c r="X1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="s">
         <v>73</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
@@ -1167,7 +1169,7 @@
         <v>32</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>32</v>
@@ -1218,15 +1220,15 @@
         <v>1</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X2" s="4"/>
       <c r="Y2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB2" t="s">
         <v>35</v>
@@ -1249,7 +1251,7 @@
         <v>32</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>32</v>
@@ -1285,7 +1287,7 @@
         <v>32</v>
       </c>
       <c r="R3" s="6">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>32</v>
@@ -1300,15 +1302,15 @@
         <v>1</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X3" s="6"/>
       <c r="Y3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z3" s="6"/>
       <c r="AA3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB3" t="s">
         <v>35</v>
@@ -1331,7 +1333,7 @@
         <v>32</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>32</v>
@@ -1382,15 +1384,15 @@
         <v>0</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X4" s="5"/>
       <c r="Y4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z4" s="5"/>
       <c r="AA4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB4" t="s">
         <v>35</v>
@@ -1464,15 +1466,15 @@
         <v>0</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X5" s="6"/>
       <c r="Y5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z5" s="6"/>
       <c r="AA5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB5" t="s">
         <v>35</v>
@@ -1546,15 +1548,15 @@
         <v>0</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X6" s="6"/>
       <c r="Y6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z6" s="6"/>
       <c r="AA6" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB6" t="s">
         <v>35</v>
@@ -1628,15 +1630,15 @@
         <v>0</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X7" s="6"/>
       <c r="Y7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z7" s="6"/>
       <c r="AA7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB7" t="s">
         <v>35</v>
@@ -1710,15 +1712,15 @@
         <v>0</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X8" s="5"/>
       <c r="Y8" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z8" s="5"/>
       <c r="AA8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB8" t="s">
         <v>35</v>
@@ -1741,7 +1743,7 @@
         <v>32</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>32</v>
@@ -1792,15 +1794,15 @@
         <v>0</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X9" s="5"/>
       <c r="Y9" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z9" s="5"/>
       <c r="AA9" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB9" t="s">
         <v>35</v>
@@ -1874,15 +1876,15 @@
         <v>0</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X10" s="5"/>
       <c r="Y10" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z10" s="5"/>
       <c r="AA10" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB10" t="s">
         <v>35</v>
@@ -1956,15 +1958,15 @@
         <v>0</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X11" s="6"/>
       <c r="Y11" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z11" s="6"/>
       <c r="AA11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB11" t="s">
         <v>35</v>
@@ -2038,19 +2040,19 @@
         <v>0</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X12" s="7">
         <v>10</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z12" s="7">
         <v>12</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB12" t="s">
         <v>35</v>
@@ -2124,19 +2126,19 @@
         <v>0</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X13" s="4">
         <v>10</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z13" s="4">
         <v>11</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB13" t="s">
         <v>35</v>
@@ -2210,15 +2212,15 @@
         <v>0</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X14" s="5"/>
       <c r="Y14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z14" s="5"/>
       <c r="AA14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB14" t="s">
         <v>35</v>
@@ -2292,15 +2294,15 @@
         <v>0</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X15" s="7"/>
       <c r="Y15" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z15" s="7"/>
       <c r="AA15" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB15" t="s">
         <v>35</v>
@@ -2374,15 +2376,15 @@
         <v>0</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X16" s="5"/>
       <c r="Y16" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z16" s="5"/>
       <c r="AA16" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB16" t="s">
         <v>35</v>
@@ -2456,15 +2458,15 @@
         <v>0</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X17" s="5"/>
       <c r="Y17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z17" s="5"/>
       <c r="AA17" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB17" t="s">
         <v>35</v>
@@ -2487,7 +2489,7 @@
         <v>32</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>32</v>
@@ -2538,15 +2540,15 @@
         <v>0</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X18" s="7"/>
       <c r="Y18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z18" s="7"/>
       <c r="AA18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB18" t="s">
         <v>35</v>
@@ -2620,15 +2622,15 @@
         <v>0</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X19" s="7"/>
       <c r="Y19" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z19" s="7"/>
       <c r="AA19" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB19" t="s">
         <v>35</v>
@@ -2702,15 +2704,15 @@
         <v>0</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X20" s="5"/>
       <c r="Y20" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z20" s="5"/>
       <c r="AA20" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB20" t="s">
         <v>35</v>
@@ -2784,15 +2786,15 @@
         <v>0</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X21" s="6"/>
       <c r="Y21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z21" s="6"/>
       <c r="AA21" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB21" t="s">
         <v>35</v>
@@ -2815,7 +2817,7 @@
         <v>32</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>32</v>
@@ -2866,15 +2868,15 @@
         <v>0</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X22" s="5"/>
       <c r="Y22" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z22" s="5"/>
       <c r="AA22" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB22" t="s">
         <v>35</v>
@@ -2948,17 +2950,17 @@
         <v>0</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X23" s="5"/>
       <c r="Y23" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z23" s="5">
         <v>40</v>
       </c>
       <c r="AA23" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB23" t="s">
         <v>35</v>
@@ -3032,15 +3034,15 @@
         <v>0</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X24" s="5"/>
       <c r="Y24" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z24" s="5"/>
       <c r="AA24" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB24" t="s">
         <v>35</v>
@@ -3114,15 +3116,15 @@
         <v>0</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X25" s="6"/>
       <c r="Y25" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z25" s="6"/>
       <c r="AA25" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB25" t="s">
         <v>35</v>
@@ -3196,17 +3198,17 @@
         <v>0</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X26" s="6">
         <v>24</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z26" s="6"/>
       <c r="AA26" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB26" t="s">
         <v>35</v>
@@ -3229,7 +3231,7 @@
         <v>32</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>32</v>
@@ -3280,17 +3282,17 @@
         <v>0</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X27" s="6">
         <v>25</v>
       </c>
       <c r="Y27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z27" s="6"/>
       <c r="AA27" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB27" t="s">
         <v>35</v>
@@ -3364,17 +3366,17 @@
         <v>0</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X28" s="4">
         <v>25</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z28" s="4"/>
       <c r="AA28" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB28" t="s">
         <v>35</v>
@@ -3448,15 +3450,15 @@
         <v>0</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X29" s="5"/>
       <c r="Y29" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z29" s="5"/>
       <c r="AA29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB29" t="s">
         <v>35</v>
@@ -3530,15 +3532,15 @@
         <v>0</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X30" s="4"/>
       <c r="Y30" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z30" s="4"/>
       <c r="AA30" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB30" t="s">
         <v>35</v>
@@ -3555,13 +3557,13 @@
         <v>32</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>67</v>
+        <v>205</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>32</v>
@@ -3603,7 +3605,7 @@
         <v>32</v>
       </c>
       <c r="T31" s="4">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="U31" s="4" t="s">
         <v>32</v>
@@ -3612,15 +3614,15 @@
         <v>0</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X31" s="4"/>
       <c r="Y31" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z31" s="4"/>
       <c r="AA31" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB31" t="s">
         <v>35</v>
@@ -3637,13 +3639,13 @@
         <v>32</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>32</v>
@@ -3694,17 +3696,17 @@
         <v>18</v>
       </c>
       <c r="W32" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X32" s="6">
         <v>52</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z32" s="6"/>
       <c r="AA32" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB32" t="s">
         <v>35</v>
@@ -3721,13 +3723,13 @@
         <v>32</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>32</v>
@@ -3778,17 +3780,17 @@
         <v>0</v>
       </c>
       <c r="W33" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X33" s="6">
         <v>12</v>
       </c>
       <c r="Y33" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z33" s="6"/>
       <c r="AA33" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB33" t="s">
         <v>35</v>
@@ -3805,13 +3807,13 @@
         <v>32</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>32</v>
@@ -3862,19 +3864,19 @@
         <v>0</v>
       </c>
       <c r="W34" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X34" s="7">
         <v>32</v>
       </c>
       <c r="Y34" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z34" s="7">
         <v>34</v>
       </c>
       <c r="AA34" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB34" t="s">
         <v>35</v>
@@ -3891,13 +3893,13 @@
         <v>32</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>32</v>
@@ -3948,19 +3950,19 @@
         <v>0</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X35" s="4">
         <v>32</v>
       </c>
       <c r="Y35" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z35" s="4">
         <v>33</v>
       </c>
       <c r="AA35" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB35" t="s">
         <v>35</v>
@@ -3977,13 +3979,13 @@
         <v>32</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>32</v>
@@ -4034,19 +4036,19 @@
         <v>0</v>
       </c>
       <c r="W36" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X36" s="5">
         <v>8</v>
       </c>
       <c r="Y36" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z36" s="5">
         <v>36</v>
       </c>
       <c r="AA36" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB36" t="s">
         <v>35</v>
@@ -4063,13 +4065,13 @@
         <v>32</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>32</v>
@@ -4120,19 +4122,19 @@
         <v>0</v>
       </c>
       <c r="W37" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X37" s="5">
         <v>8</v>
       </c>
       <c r="Y37" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z37" s="5">
         <v>35</v>
       </c>
       <c r="AA37" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB37" t="s">
         <v>35</v>
@@ -4149,13 +4151,13 @@
         <v>32</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>32</v>
@@ -4206,17 +4208,17 @@
         <v>0</v>
       </c>
       <c r="W38" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X38" s="5">
         <v>39</v>
       </c>
       <c r="Y38" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z38" s="5"/>
       <c r="AA38" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB38" t="s">
         <v>35</v>
@@ -4233,13 +4235,13 @@
         <v>32</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>32</v>
@@ -4290,17 +4292,17 @@
         <v>0</v>
       </c>
       <c r="W39" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X39" s="5">
         <v>37</v>
       </c>
       <c r="Y39" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z39" s="5"/>
       <c r="AA39" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB39" t="s">
         <v>35</v>
@@ -4317,13 +4319,13 @@
         <v>32</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>32</v>
@@ -4374,17 +4376,17 @@
         <v>0</v>
       </c>
       <c r="W40" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X40" s="5">
         <v>21</v>
       </c>
       <c r="Y40" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z40" s="5"/>
       <c r="AA40" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB40" t="s">
         <v>35</v>
@@ -4401,13 +4403,13 @@
         <v>32</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>32</v>
@@ -4458,17 +4460,17 @@
         <v>0</v>
       </c>
       <c r="W41" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X41" s="5"/>
       <c r="Y41" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z41" s="5">
         <v>22</v>
       </c>
       <c r="AA41" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB41" t="s">
         <v>35</v>
@@ -4485,13 +4487,13 @@
         <v>32</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>32</v>
@@ -4542,15 +4544,15 @@
         <v>0</v>
       </c>
       <c r="W42" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X42" s="5"/>
       <c r="Y42" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z42" s="5"/>
       <c r="AA42" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB42" t="s">
         <v>35</v>
@@ -4567,13 +4569,13 @@
         <v>32</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>32</v>
@@ -4624,15 +4626,15 @@
         <v>0</v>
       </c>
       <c r="W43" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X43" s="5"/>
       <c r="Y43" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z43" s="5"/>
       <c r="AA43" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB43" t="s">
         <v>35</v>
@@ -4649,13 +4651,13 @@
         <v>32</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>32</v>
@@ -4706,15 +4708,15 @@
         <v>0</v>
       </c>
       <c r="W44" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X44" s="5"/>
       <c r="Y44" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z44" s="5"/>
       <c r="AA44" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB44" t="s">
         <v>35</v>
@@ -4731,13 +4733,13 @@
         <v>32</v>
       </c>
       <c r="D45" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>32</v>
@@ -4788,15 +4790,15 @@
         <v>0</v>
       </c>
       <c r="W45" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X45" s="5"/>
       <c r="Y45" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z45" s="5"/>
       <c r="AA45" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB45" t="s">
         <v>35</v>
@@ -4813,13 +4815,13 @@
         <v>32</v>
       </c>
       <c r="D46" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>32</v>
@@ -4870,17 +4872,17 @@
         <v>0</v>
       </c>
       <c r="W46" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X46" s="5">
         <v>19</v>
       </c>
       <c r="Y46" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z46" s="5"/>
       <c r="AA46" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB46" t="s">
         <v>35</v>
@@ -4897,13 +4899,13 @@
         <v>32</v>
       </c>
       <c r="D47" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>32</v>
@@ -4954,17 +4956,17 @@
         <v>0</v>
       </c>
       <c r="W47" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X47" s="5">
         <v>46</v>
       </c>
       <c r="Y47" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z47" s="5"/>
       <c r="AA47" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB47" t="s">
         <v>35</v>
@@ -4981,13 +4983,13 @@
         <v>32</v>
       </c>
       <c r="D48" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>32</v>
@@ -5038,17 +5040,17 @@
         <v>0</v>
       </c>
       <c r="W48" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X48" s="5">
         <v>47</v>
       </c>
       <c r="Y48" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z48" s="5"/>
       <c r="AA48" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB48" t="s">
         <v>35</v>
@@ -5065,13 +5067,13 @@
         <v>32</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>32</v>
@@ -5122,17 +5124,17 @@
         <v>0</v>
       </c>
       <c r="W49" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X49" s="5">
         <v>48</v>
       </c>
       <c r="Y49" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z49" s="5"/>
       <c r="AA49" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB49" t="s">
         <v>35</v>
@@ -5149,13 +5151,13 @@
         <v>32</v>
       </c>
       <c r="D50" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>115</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>32</v>
@@ -5206,17 +5208,17 @@
         <v>0</v>
       </c>
       <c r="W50" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X50" s="6">
         <v>26</v>
       </c>
       <c r="Y50" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z50" s="6"/>
       <c r="AA50" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB50" t="s">
         <v>35</v>
@@ -5233,13 +5235,13 @@
         <v>32</v>
       </c>
       <c r="D51" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>32</v>
@@ -5290,17 +5292,17 @@
         <v>0</v>
       </c>
       <c r="W51" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X51" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y51" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z51" s="6"/>
       <c r="AA51" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB51" t="s">
         <v>35</v>
@@ -5317,13 +5319,13 @@
         <v>32</v>
       </c>
       <c r="D52" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>32</v>
@@ -5374,17 +5376,17 @@
         <v>0</v>
       </c>
       <c r="W52" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X52" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Y52" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z52" s="6"/>
       <c r="AA52" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB52" t="s">
         <v>35</v>
@@ -5401,13 +5403,13 @@
         <v>32</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>32</v>
@@ -5425,13 +5427,13 @@
         <v>32</v>
       </c>
       <c r="L53" s="6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="M53" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N53" s="6">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="O53" s="6" t="s">
         <v>32</v>
@@ -5458,15 +5460,15 @@
         <v>7</v>
       </c>
       <c r="W53" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X53" s="6"/>
       <c r="Y53" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z53" s="6"/>
       <c r="AA53" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB53" t="s">
         <v>35</v>
@@ -5483,13 +5485,13 @@
         <v>32</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>32</v>
@@ -5501,13 +5503,13 @@
         <v>32</v>
       </c>
       <c r="J54" s="4">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>32</v>
       </c>
       <c r="L54" s="4">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="M54" s="4" t="s">
         <v>32</v>
@@ -5540,15 +5542,15 @@
         <v>7</v>
       </c>
       <c r="W54" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X54" s="4"/>
       <c r="Y54" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z54" s="4"/>
       <c r="AA54" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB54" t="s">
         <v>35</v>
@@ -5565,13 +5567,13 @@
         <v>32</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>32</v>
@@ -5622,15 +5624,15 @@
         <v>0</v>
       </c>
       <c r="W55" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X55" s="4"/>
       <c r="Y55" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z55" s="4"/>
       <c r="AA55" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB55" t="s">
         <v>35</v>
@@ -5647,13 +5649,13 @@
         <v>32</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>32</v>
@@ -5704,15 +5706,15 @@
         <v>0</v>
       </c>
       <c r="W56" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X56" s="4"/>
       <c r="Y56" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z56" s="4"/>
       <c r="AA56" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB56" t="s">
         <v>35</v>
@@ -5729,13 +5731,13 @@
         <v>32</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>32</v>
@@ -5786,15 +5788,15 @@
         <v>0</v>
       </c>
       <c r="W57" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X57" s="4"/>
       <c r="Y57" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z57" s="4"/>
       <c r="AA57" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB57" t="s">
         <v>35</v>
@@ -5811,13 +5813,13 @@
         <v>32</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>32</v>
@@ -5868,17 +5870,17 @@
         <v>0</v>
       </c>
       <c r="W58" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X58" s="6">
         <v>52</v>
       </c>
       <c r="Y58" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z58" s="6"/>
       <c r="AA58" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB58" t="s">
         <v>35</v>
@@ -5895,13 +5897,13 @@
         <v>32</v>
       </c>
       <c r="D59" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>32</v>
@@ -5952,15 +5954,15 @@
         <v>0</v>
       </c>
       <c r="W59" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X59" s="4"/>
       <c r="Y59" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z59" s="4"/>
       <c r="AA59" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB59" t="s">
         <v>35</v>
@@ -5977,13 +5979,13 @@
         <v>32</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>32</v>
@@ -6034,15 +6036,15 @@
         <v>0</v>
       </c>
       <c r="W60" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X60" s="6"/>
       <c r="Y60" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z60" s="6"/>
       <c r="AA60" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB60" t="s">
         <v>35</v>
@@ -6059,13 +6061,13 @@
         <v>32</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>32</v>
@@ -6116,15 +6118,15 @@
         <v>0</v>
       </c>
       <c r="W61" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X61" s="4"/>
       <c r="Y61" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z61" s="4"/>
       <c r="AA61" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB61" t="s">
         <v>35</v>
@@ -6141,13 +6143,13 @@
         <v>32</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>32</v>
@@ -6198,15 +6200,15 @@
         <v>0</v>
       </c>
       <c r="W62" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X62" s="4"/>
       <c r="Y62" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z62" s="4"/>
       <c r="AA62" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB62" t="s">
         <v>35</v>
@@ -6223,13 +6225,13 @@
         <v>32</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>32</v>
@@ -6280,15 +6282,15 @@
         <v>0</v>
       </c>
       <c r="W63" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X63" s="4"/>
       <c r="Y63" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z63" s="4"/>
       <c r="AA63" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB63" t="s">
         <v>35</v>
@@ -6305,13 +6307,13 @@
         <v>32</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>32</v>
@@ -6362,15 +6364,15 @@
         <v>0</v>
       </c>
       <c r="W64" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X64" s="4"/>
       <c r="Y64" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z64" s="4"/>
       <c r="AA64" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB64" t="s">
         <v>35</v>
@@ -6387,13 +6389,13 @@
         <v>32</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>32</v>
@@ -6444,15 +6446,15 @@
         <v>0</v>
       </c>
       <c r="W65" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X65" s="4"/>
       <c r="Y65" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z65" s="4"/>
       <c r="AA65" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB65" t="s">
         <v>35</v>
@@ -6469,13 +6471,13 @@
         <v>32</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>32</v>
@@ -6526,15 +6528,15 @@
         <v>0</v>
       </c>
       <c r="W66" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X66" s="4"/>
       <c r="Y66" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z66" s="4"/>
       <c r="AA66" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB66" t="s">
         <v>35</v>
@@ -6551,13 +6553,13 @@
         <v>32</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>32</v>
@@ -6608,15 +6610,15 @@
         <v>0</v>
       </c>
       <c r="W67" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X67" s="4"/>
       <c r="Y67" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z67" s="4"/>
       <c r="AA67" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB67" t="s">
         <v>35</v>
@@ -6633,13 +6635,13 @@
         <v>32</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>32</v>
@@ -6690,17 +6692,17 @@
         <v>0</v>
       </c>
       <c r="W68" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X68" s="4">
         <v>66</v>
       </c>
       <c r="Y68" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z68" s="4"/>
       <c r="AA68" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB68" t="s">
         <v>35</v>
@@ -6717,13 +6719,13 @@
         <v>32</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>32</v>
@@ -6774,15 +6776,15 @@
         <v>0</v>
       </c>
       <c r="W69" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X69" s="4"/>
       <c r="Y69" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z69" s="4"/>
       <c r="AA69" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB69" t="s">
         <v>35</v>
@@ -6799,13 +6801,13 @@
         <v>32</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>32</v>
@@ -6856,17 +6858,17 @@
         <v>0</v>
       </c>
       <c r="W70" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X70" s="4">
         <v>68</v>
       </c>
       <c r="Y70" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z70" s="4"/>
       <c r="AA70" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB70" t="s">
         <v>35</v>
@@ -6883,13 +6885,13 @@
         <v>32</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>32</v>
@@ -6940,15 +6942,15 @@
         <v>0</v>
       </c>
       <c r="W71" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X71" s="5"/>
       <c r="Y71" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z71" s="5"/>
       <c r="AA71" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB71" t="s">
         <v>35</v>
@@ -6965,13 +6967,13 @@
         <v>32</v>
       </c>
       <c r="D72" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F72" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>32</v>
@@ -7022,15 +7024,15 @@
         <v>0</v>
       </c>
       <c r="W72" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X72" s="5"/>
       <c r="Y72" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z72" s="5"/>
       <c r="AA72" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB72" t="s">
         <v>35</v>
@@ -7047,13 +7049,13 @@
         <v>32</v>
       </c>
       <c r="D73" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F73" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>32</v>
@@ -7104,15 +7106,15 @@
         <v>0</v>
       </c>
       <c r="W73" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X73" s="5"/>
       <c r="Y73" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z73" s="5"/>
       <c r="AA73" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB73" t="s">
         <v>35</v>
@@ -7129,13 +7131,13 @@
         <v>32</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>32</v>
@@ -7186,15 +7188,15 @@
         <v>0</v>
       </c>
       <c r="W74" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X74" s="5"/>
       <c r="Y74" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z74" s="5"/>
       <c r="AA74" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB74" t="s">
         <v>35</v>
@@ -7211,13 +7213,13 @@
         <v>32</v>
       </c>
       <c r="D75" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>32</v>
@@ -7268,15 +7270,15 @@
         <v>0</v>
       </c>
       <c r="W75" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X75" s="4"/>
       <c r="Y75" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z75" s="4"/>
       <c r="AA75" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB75" t="s">
         <v>35</v>
@@ -7293,13 +7295,13 @@
         <v>32</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>32</v>
@@ -7350,15 +7352,15 @@
         <v>0</v>
       </c>
       <c r="W76" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X76" s="4"/>
       <c r="Y76" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z76" s="4"/>
       <c r="AA76" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB76" t="s">
         <v>35</v>
@@ -7375,13 +7377,13 @@
         <v>32</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>32</v>
@@ -7432,17 +7434,17 @@
         <v>0</v>
       </c>
       <c r="W77" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X77" s="4">
         <v>77</v>
       </c>
       <c r="Y77" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z77" s="4"/>
       <c r="AA77" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB77" t="s">
         <v>35</v>
@@ -7459,13 +7461,13 @@
         <v>32</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>32</v>
@@ -7516,15 +7518,15 @@
         <v>0</v>
       </c>
       <c r="W78" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X78" s="4"/>
       <c r="Y78" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z78" s="4"/>
       <c r="AA78" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB78" t="s">
         <v>35</v>
@@ -7541,13 +7543,13 @@
         <v>32</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>32</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>32</v>
@@ -7598,15 +7600,15 @@
         <v>0</v>
       </c>
       <c r="W79" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X79" s="9"/>
       <c r="Y79" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z79" s="9"/>
       <c r="AA79" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB79" t="s">
         <v>35</v>
@@ -7623,13 +7625,13 @@
         <v>32</v>
       </c>
       <c r="D80" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>32</v>
@@ -7680,15 +7682,15 @@
         <v>14</v>
       </c>
       <c r="W80" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X80" s="9"/>
       <c r="Y80" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z80" s="9"/>
       <c r="AA80" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB80" t="s">
         <v>35</v>
@@ -7705,13 +7707,13 @@
         <v>32</v>
       </c>
       <c r="D81" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F81" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>32</v>
@@ -7762,15 +7764,15 @@
         <v>0</v>
       </c>
       <c r="W81" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X81" s="6"/>
       <c r="Y81" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z81" s="6"/>
       <c r="AA81" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB81" t="s">
         <v>35</v>
@@ -7787,13 +7789,13 @@
         <v>32</v>
       </c>
       <c r="D82" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F82" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="G82" s="6" t="s">
         <v>32</v>
@@ -7844,15 +7846,15 @@
         <v>0</v>
       </c>
       <c r="W82" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X82" s="6"/>
       <c r="Y82" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z82" s="6"/>
       <c r="AA82" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB82" t="s">
         <v>35</v>
@@ -7869,13 +7871,13 @@
         <v>32</v>
       </c>
       <c r="D83" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F83" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="G83" s="6" t="s">
         <v>32</v>
@@ -7926,15 +7928,15 @@
         <v>81</v>
       </c>
       <c r="W83" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X83" s="6"/>
       <c r="Y83" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z83" s="6"/>
       <c r="AA83" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB83" t="s">
         <v>35</v>
@@ -7951,13 +7953,13 @@
         <v>32</v>
       </c>
       <c r="D84" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F84" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>171</v>
       </c>
       <c r="G84" s="6" t="s">
         <v>32</v>
@@ -8008,15 +8010,15 @@
         <v>82</v>
       </c>
       <c r="W84" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X84" s="6"/>
       <c r="Y84" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z84" s="6"/>
       <c r="AA84" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB84" t="s">
         <v>35</v>
@@ -8033,13 +8035,13 @@
         <v>32</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G85" s="6" t="s">
         <v>32</v>
@@ -8090,15 +8092,15 @@
         <v>83</v>
       </c>
       <c r="W85" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X85" s="6"/>
       <c r="Y85" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z85" s="6"/>
       <c r="AA85" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB85" t="s">
         <v>35</v>
@@ -8115,13 +8117,13 @@
         <v>32</v>
       </c>
       <c r="D86" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>32</v>
@@ -8172,15 +8174,15 @@
         <v>83</v>
       </c>
       <c r="W86" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X86" s="4"/>
       <c r="Y86" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z86" s="4"/>
       <c r="AA86" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB86" t="s">
         <v>35</v>
@@ -8197,13 +8199,13 @@
         <v>32</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G87" s="6" t="s">
         <v>32</v>
@@ -8254,15 +8256,15 @@
         <v>0</v>
       </c>
       <c r="W87" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X87" s="6"/>
       <c r="Y87" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z87" s="6"/>
       <c r="AA87" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB87" t="s">
         <v>35</v>
@@ -8279,13 +8281,13 @@
         <v>32</v>
       </c>
       <c r="D88" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F88" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>32</v>
@@ -8336,15 +8338,15 @@
         <v>0</v>
       </c>
       <c r="W88" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X88" s="6"/>
       <c r="Y88" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z88" s="6"/>
       <c r="AA88" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB88" t="s">
         <v>35</v>
@@ -8361,13 +8363,13 @@
         <v>32</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>32</v>
@@ -8418,15 +8420,15 @@
         <v>0</v>
       </c>
       <c r="W89" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X89" s="6"/>
       <c r="Y89" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z89" s="6"/>
       <c r="AA89" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB89" t="s">
         <v>35</v>
@@ -8443,13 +8445,13 @@
         <v>32</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>32</v>
@@ -8500,15 +8502,15 @@
         <v>88</v>
       </c>
       <c r="W90" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X90" s="6"/>
       <c r="Y90" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z90" s="6"/>
       <c r="AA90" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB90" t="s">
         <v>35</v>
@@ -8525,13 +8527,13 @@
         <v>32</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>32</v>
@@ -8582,15 +8584,15 @@
         <v>89</v>
       </c>
       <c r="W91" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X91" s="6"/>
       <c r="Y91" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z91" s="6"/>
       <c r="AA91" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB91" t="s">
         <v>35</v>

</xml_diff>